<commit_message>
cambio del atributo r4grp112. modificado el diseño del configuration2.tml. se ha cambiado el comportamiento del modal
</commit_message>
<xml_diff>
--- a/doc/ParametrosConfig.xlsx
+++ b/doc/ParametrosConfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="650">
   <si>
     <t>RES14CNT_GN</t>
   </si>
@@ -1956,6 +1956,54 @@
   </si>
   <si>
     <t>enableSegmentCh</t>
+  </si>
+  <si>
+    <t>R4CN704</t>
+  </si>
+  <si>
+    <t>enableMeteorology</t>
+  </si>
+  <si>
+    <t>Habilitar meteorología</t>
+  </si>
+  <si>
+    <t>standardPrint</t>
+  </si>
+  <si>
+    <t>Decmales en cantXart</t>
+  </si>
+  <si>
+    <t>decimalArt</t>
+  </si>
+  <si>
+    <t>printKitchenCalif</t>
+  </si>
+  <si>
+    <t>printer1</t>
+  </si>
+  <si>
+    <t>printer2</t>
+  </si>
+  <si>
+    <t>printerEsp</t>
+  </si>
+  <si>
+    <t>Printer 1</t>
+  </si>
+  <si>
+    <t>Printer 2</t>
+  </si>
+  <si>
+    <t>Printer Especial</t>
+  </si>
+  <si>
+    <t>R4CNT142</t>
+  </si>
+  <si>
+    <t>R4CNT143</t>
+  </si>
+  <si>
+    <t>R4CNT141</t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2065,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2060,11 +2108,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2093,9 +2159,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2111,6 +2174,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2407,8 +2480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="F134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H141" sqref="H141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2425,29 +2498,29 @@
     <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" customWidth="1"/>
     <col min="29" max="29" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="J1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="2" t="s">
@@ -2467,13 +2540,13 @@
         <v>5</v>
       </c>
       <c r="X1" s="3"/>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
     </row>
     <row r="2" spans="1:29">
       <c r="B2" s="4" t="s">
@@ -2860,20 +2933,20 @@
       <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>605</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>0</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="18"/>
+      <c r="H7" s="17" t="s">
         <v>66</v>
       </c>
       <c r="J7" s="4">
@@ -3503,7 +3576,7 @@
       <c r="D17" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <v>1.35067</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -3619,20 +3692,20 @@
       <c r="B19" s="4">
         <v>17</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>607</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>598</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="15">
         <v>1020</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16" t="s">
+      <c r="G19" s="14"/>
+      <c r="H19" s="15" t="s">
         <v>599</v>
       </c>
       <c r="I19" s="3"/>
@@ -3739,19 +3812,19 @@
       <c r="B21" s="4">
         <v>19</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>608</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <v>1021</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="13" t="s">
         <v>601</v>
       </c>
@@ -3817,7 +3890,7 @@
         <v>178</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="21">
+      <c r="J22" s="20">
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
@@ -3851,20 +3924,20 @@
       <c r="B23" s="4">
         <v>21</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>609</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>602</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="14">
         <v>1023</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
       <c r="I23" s="3"/>
       <c r="J23" s="4">
         <v>21</v>
@@ -3925,6 +3998,24 @@
         <v>186</v>
       </c>
       <c r="I24" s="3"/>
+      <c r="J24" s="20">
+        <v>22</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="M24" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>636</v>
+      </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="2" t="s">
@@ -3945,28 +4036,45 @@
       </c>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="2:24">
+    <row r="25" spans="2:24" ht="22.5">
       <c r="B25" s="4">
         <v>23</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>610</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>603</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>1024</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="17" t="s">
+      <c r="G25" s="14"/>
+      <c r="H25" s="16" t="s">
         <v>604</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="J25" s="20">
+        <v>23</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="Q25" s="3"/>
       <c r="R25" s="2" t="s">
         <v>222</v>
@@ -4007,6 +4115,24 @@
         <v>196</v>
       </c>
       <c r="I26" s="3"/>
+      <c r="J26" s="20">
+        <v>24</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>638</v>
+      </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="2" t="s">
@@ -4048,7 +4174,25 @@
         <v>204</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="P27" s="3"/>
+      <c r="J27" s="20">
+        <v>25</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P27" s="2"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="2" t="s">
         <v>55</v>
@@ -4091,6 +4235,24 @@
         <v>212</v>
       </c>
       <c r="I28" s="3"/>
+      <c r="J28" s="20">
+        <v>26</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="M28" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>644</v>
+      </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="2" t="s">
@@ -4132,6 +4294,24 @@
         <v>218</v>
       </c>
       <c r="I29" s="3"/>
+      <c r="J29" s="20">
+        <v>27</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>645</v>
+      </c>
       <c r="R29" s="2" t="s">
         <v>240</v>
       </c>
@@ -4171,6 +4351,24 @@
         <v>225</v>
       </c>
       <c r="I30" s="3"/>
+      <c r="J30" s="20">
+        <v>28</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>646</v>
+      </c>
       <c r="R30" s="2" t="s">
         <v>65</v>
       </c>
@@ -6120,6 +6318,28 @@
         <v>413</v>
       </c>
       <c r="I68" s="3"/>
+      <c r="J68" s="20">
+        <v>22</v>
+      </c>
+      <c r="K68" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="M68" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="O68" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P68" t="str">
+        <f>CONCATENATE(J68,K68,L68,M68,N68,O68)</f>
+        <v>22,"R4CN704","enableMeteorology","false"</v>
+      </c>
       <c r="R68" s="2" t="s">
         <v>426</v>
       </c>
@@ -6162,6 +6382,28 @@
         <v>417</v>
       </c>
       <c r="I69" s="3"/>
+      <c r="J69" s="20">
+        <v>23</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L69" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="M69" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N69" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="O69" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P69" t="str">
+        <f>CONCATENATE(J69,K69,L69,M69,N69,O69)</f>
+        <v>23,"RSCNT033","standardPrint","false"</v>
+      </c>
       <c r="R69" s="2" t="s">
         <v>430</v>
       </c>
@@ -6200,6 +6442,28 @@
         <v>421</v>
       </c>
       <c r="I70" s="3"/>
+      <c r="J70" s="20">
+        <v>24</v>
+      </c>
+      <c r="K70" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L70" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="M70" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>639</v>
+      </c>
+      <c r="O70" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P70" t="str">
+        <f t="shared" ref="P70:P74" si="1">CONCATENATE(J70,K70,L70,M70,N70,O70)</f>
+        <v>24,"RSCNT025","decimalArt","false"</v>
+      </c>
       <c r="R70" s="2" t="s">
         <v>434</v>
       </c>
@@ -6240,6 +6504,28 @@
         <v>425</v>
       </c>
       <c r="I71" s="3"/>
+      <c r="J71" s="20">
+        <v>25</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M71" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N71" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O71" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P71" t="str">
+        <f t="shared" si="1"/>
+        <v>25,"R4CNT043","printKitchenCalif","false"</v>
+      </c>
       <c r="R71" s="2" t="s">
         <v>438</v>
       </c>
@@ -6278,6 +6564,28 @@
         <v>429</v>
       </c>
       <c r="I72" s="3"/>
+      <c r="J72" s="20">
+        <v>26</v>
+      </c>
+      <c r="K72" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="M72" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="O72" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P72" t="str">
+        <f t="shared" si="1"/>
+        <v>26,"R4CNT141","printer1","false"</v>
+      </c>
       <c r="R72" s="2" t="s">
         <v>442</v>
       </c>
@@ -6320,6 +6628,28 @@
         <v>433</v>
       </c>
       <c r="I73" s="3"/>
+      <c r="J73" s="20">
+        <v>27</v>
+      </c>
+      <c r="K73" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L73" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="M73" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="O73" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P73" t="str">
+        <f t="shared" si="1"/>
+        <v>27,"R4CNT142","printer2","false"</v>
+      </c>
       <c r="R73" s="2" t="s">
         <v>446</v>
       </c>
@@ -6358,6 +6688,28 @@
         <v>437</v>
       </c>
       <c r="I74" s="3"/>
+      <c r="J74" s="20">
+        <v>28</v>
+      </c>
+      <c r="K74" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="M74" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="O74" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="P74" t="str">
+        <f t="shared" si="1"/>
+        <v>28,"R4CNT143","printerEsp","false"</v>
+      </c>
       <c r="R74" s="2" t="s">
         <v>452</v>
       </c>
@@ -7648,7 +8000,7 @@
         <v>628</v>
       </c>
       <c r="K133" t="str">
-        <f t="shared" ref="K133:K196" si="1">CONCATENATE(B133,C133,D133,E133,F133,G133,H133,I133)</f>
+        <f t="shared" ref="K133:K196" si="2">CONCATENATE(B133,C133,D133,E133,F133,G133,H133,I133)</f>
         <v>3,"R4CNT013_03","lastCommand","0"</v>
       </c>
     </row>
@@ -7678,7 +8030,7 @@
         <v>628</v>
       </c>
       <c r="K134" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4,"R4CNT013_04","lastClient","0"</v>
       </c>
     </row>
@@ -7689,26 +8041,26 @@
       <c r="C135" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D135" s="18" t="s">
+      <c r="D135" s="17" t="s">
         <v>606</v>
       </c>
       <c r="E135" t="s">
         <v>220</v>
       </c>
-      <c r="F135" s="19" t="s">
+      <c r="F135" s="18" t="s">
         <v>605</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H135" s="19">
+      <c r="H135" s="18">
         <v>0</v>
       </c>
       <c r="I135" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K135" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5,"R4CNT013_05","numNotaFis","0"</v>
       </c>
     </row>
@@ -7738,7 +8090,7 @@
         <v>628</v>
       </c>
       <c r="K136" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6,"R4CNT002","restCateg"," "</v>
       </c>
     </row>
@@ -7768,7 +8120,7 @@
         <v>628</v>
       </c>
       <c r="K137" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7,"R4CNT004","tableNumber","342"</v>
       </c>
     </row>
@@ -7798,7 +8150,7 @@
         <v>628</v>
       </c>
       <c r="K138" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8,"R4CNT006","covServCharImp"," "</v>
       </c>
     </row>
@@ -7828,7 +8180,7 @@
         <v>628</v>
       </c>
       <c r="K139" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9,"R4CNT106","covServCharIVAType","1"</v>
       </c>
     </row>
@@ -7858,7 +8210,7 @@
         <v>628</v>
       </c>
       <c r="K140" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10,"RSCNT031","literalCharCov","Pan, Cubiertos y Servicio Mesa"</v>
       </c>
     </row>
@@ -7882,14 +8234,14 @@
         <v>220</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="I141" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K141" t="str">
-        <f t="shared" si="1"/>
-        <v>11,"R4CNT008","tipWaiterInvoice%","""</v>
+        <f t="shared" si="2"/>
+        <v>11,"R4CNT008","tipWaiterInvoice%"," "</v>
       </c>
     </row>
     <row r="142" spans="2:11" ht="22.5">
@@ -7918,7 +8270,7 @@
         <v>628</v>
       </c>
       <c r="K142" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12,"R4CNT108","tipWaiterInvoiceIVA","1"</v>
       </c>
     </row>
@@ -7948,7 +8300,7 @@
         <v>628</v>
       </c>
       <c r="K143" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13,"RSCNT032","literalTipsAuto","Servicio Inluido en Factura"</v>
       </c>
     </row>
@@ -7978,7 +8330,7 @@
         <v>628</v>
       </c>
       <c r="K144" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14,"R4CNT012","actualSessionDate","20130201"</v>
       </c>
     </row>
@@ -8001,14 +8353,14 @@
       <c r="G145" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H145" s="20">
+      <c r="H145" s="19">
         <v>1.35067</v>
       </c>
       <c r="I145" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K145" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15,"R4CNT102","eurUSDChange","1,35067"</v>
       </c>
     </row>
@@ -8038,7 +8390,7 @@
         <v>628</v>
       </c>
       <c r="K146" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16,"R4CNT202","breakfastServHot","DESA"</v>
       </c>
     </row>
@@ -8049,26 +8401,26 @@
       <c r="C147" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D147" s="16" t="s">
+      <c r="D147" s="15" t="s">
         <v>607</v>
       </c>
       <c r="E147" t="s">
         <v>220</v>
       </c>
-      <c r="F147" s="16" t="s">
+      <c r="F147" s="15" t="s">
         <v>598</v>
       </c>
       <c r="G147" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H147" s="16">
+      <c r="H147" s="15">
         <v>1020</v>
       </c>
       <c r="I147" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K147" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17,"R4CNT202_01","breakfastServCode","1020"</v>
       </c>
     </row>
@@ -8098,7 +8450,7 @@
         <v>628</v>
       </c>
       <c r="K148" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18,"R4CNT203","lunchServHotel","ALMU"</v>
       </c>
     </row>
@@ -8109,26 +8461,26 @@
       <c r="C149" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D149" s="16" t="s">
+      <c r="D149" s="15" t="s">
         <v>608</v>
       </c>
       <c r="E149" t="s">
         <v>220</v>
       </c>
-      <c r="F149" s="16" t="s">
+      <c r="F149" s="15" t="s">
         <v>600</v>
       </c>
       <c r="G149" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H149" s="16">
+      <c r="H149" s="15">
         <v>1021</v>
       </c>
       <c r="I149" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K149" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19,"R4CNT203_01","lunchServCode","1021"</v>
       </c>
     </row>
@@ -8158,7 +8510,7 @@
         <v>628</v>
       </c>
       <c r="K150" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20,"R4CNT204","dinnerServHotel","CENA"</v>
       </c>
     </row>
@@ -8169,26 +8521,26 @@
       <c r="C151" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D151" s="16" t="s">
+      <c r="D151" s="15" t="s">
         <v>609</v>
       </c>
       <c r="E151" t="s">
         <v>220</v>
       </c>
-      <c r="F151" s="16" t="s">
+      <c r="F151" s="15" t="s">
         <v>602</v>
       </c>
       <c r="G151" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H151" s="15">
+      <c r="H151" s="14">
         <v>1023</v>
       </c>
       <c r="I151" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K151" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21,"R4CNT204_01","dinnerServCode","1023"</v>
       </c>
     </row>
@@ -8218,7 +8570,7 @@
         <v>628</v>
       </c>
       <c r="K152" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22,"R4CNT205","otherServHotel","EVEN"</v>
       </c>
     </row>
@@ -8229,26 +8581,26 @@
       <c r="C153" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D153" s="16" t="s">
+      <c r="D153" s="15" t="s">
         <v>610</v>
       </c>
       <c r="E153" t="s">
         <v>220</v>
       </c>
-      <c r="F153" s="16" t="s">
+      <c r="F153" s="15" t="s">
         <v>603</v>
       </c>
       <c r="G153" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H153" s="15">
+      <c r="H153" s="14">
         <v>1024</v>
       </c>
       <c r="I153" s="3" t="s">
         <v>628</v>
       </c>
       <c r="K153" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23,"R4CNT205_01","otherServCode","1024"</v>
       </c>
     </row>
@@ -8278,7 +8630,7 @@
         <v>628</v>
       </c>
       <c r="K154" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24,"R4CNT041","integrationHotel","N"</v>
       </c>
     </row>
@@ -8308,7 +8660,7 @@
         <v>628</v>
       </c>
       <c r="K155" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25,"R4CNT707","cancelTableLevel","0"</v>
       </c>
     </row>
@@ -8338,7 +8690,7 @@
         <v>628</v>
       </c>
       <c r="K156" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26,"R4CNT706","dayMenuLevel","0"</v>
       </c>
     </row>
@@ -8368,7 +8720,7 @@
         <v>628</v>
       </c>
       <c r="K157" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27,"RSCNT029","literalEspBill","Menú del día"</v>
       </c>
     </row>
@@ -8398,7 +8750,7 @@
         <v>628</v>
       </c>
       <c r="K158" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28,"R4CNT348","assocElemTips","8899"</v>
       </c>
     </row>
@@ -8428,7 +8780,7 @@
         <v>628</v>
       </c>
       <c r="K159" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29,"R4CNT350","assocElemDto1","8903"</v>
       </c>
     </row>
@@ -8458,7 +8810,7 @@
         <v>628</v>
       </c>
       <c r="K160" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30,"R4CNT351","assocElemDto1%","3.00"</v>
       </c>
     </row>
@@ -8488,7 +8840,7 @@
         <v>628</v>
       </c>
       <c r="K161" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31,"R4CNT353","assocElemDto2","8907"</v>
       </c>
     </row>
@@ -8518,7 +8870,7 @@
         <v>628</v>
       </c>
       <c r="K162" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32,"R4CNT354","assocElemDto2%","7.00"</v>
       </c>
     </row>
@@ -8548,7 +8900,7 @@
         <v>628</v>
       </c>
       <c r="K163" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33,"R4CNT356","assocElemDto3","8910"</v>
       </c>
     </row>
@@ -8578,7 +8930,7 @@
         <v>628</v>
       </c>
       <c r="K164" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34,"R4CNT357","assocElemDto3%","10.00"</v>
       </c>
     </row>
@@ -8608,7 +8960,7 @@
         <v>628</v>
       </c>
       <c r="K165" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35,"R4CNT358","assocElemTPV","7000"</v>
       </c>
     </row>
@@ -8638,7 +8990,7 @@
         <v>628</v>
       </c>
       <c r="K166" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36,"R4CNT359","chargeTPV","50"</v>
       </c>
     </row>
@@ -8668,7 +9020,7 @@
         <v>628</v>
       </c>
       <c r="K167" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37,"R4CNT047","fieldSeparator",";"</v>
       </c>
     </row>
@@ -8698,7 +9050,7 @@
         <v>628</v>
       </c>
       <c r="K168" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38,"R4CNT048","alphabSeparator","“"</v>
       </c>
     </row>
@@ -8728,7 +9080,7 @@
         <v>628</v>
       </c>
       <c r="K169" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39,"RSCNT003","colCommand","#CCCCCC"</v>
       </c>
     </row>
@@ -8758,7 +9110,7 @@
         <v>628</v>
       </c>
       <c r="K170" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40,"RSCNT303","colBackground","#B2ACAB"</v>
       </c>
     </row>
@@ -8788,7 +9140,7 @@
         <v>628</v>
       </c>
       <c r="K171" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41,"RSCNT004","colBill","#CCCCCC"</v>
       </c>
     </row>
@@ -8818,7 +9170,7 @@
         <v>628</v>
       </c>
       <c r="K172" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42,"RSCNT304","colBackground2","#6C6C6C"</v>
       </c>
     </row>
@@ -8848,7 +9200,7 @@
         <v>628</v>
       </c>
       <c r="K173" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43,"RSCNT005","colCharge","#CCCCCC"</v>
       </c>
     </row>
@@ -8878,7 +9230,7 @@
         <v>628</v>
       </c>
       <c r="K174" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44,"RSCNT006","colTrasp","#CCCCCC"</v>
       </c>
     </row>
@@ -8908,7 +9260,7 @@
         <v>628</v>
       </c>
       <c r="K175" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45,"RSCNT007","colTabEmpty","#CCCCCC"</v>
       </c>
     </row>
@@ -8938,7 +9290,7 @@
         <v>628</v>
       </c>
       <c r="K176" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46,"RSCNT008","colTabBusy","#CCCCCC"</v>
       </c>
     </row>
@@ -8968,7 +9320,7 @@
         <v>628</v>
       </c>
       <c r="K177" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47,"RSCNT009","colTabAtached","#CCCCCC"</v>
       </c>
     </row>
@@ -8998,7 +9350,7 @@
         <v>628</v>
       </c>
       <c r="K178" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48,"RSCNT010","colTabReserved","#CCCCCC"</v>
       </c>
     </row>
@@ -9028,7 +9380,7 @@
         <v>628</v>
       </c>
       <c r="K179" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49,"RSCNT011","colTabBill","#CCCCCC"</v>
       </c>
     </row>
@@ -9058,7 +9410,7 @@
         <v>628</v>
       </c>
       <c r="K180" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50,"RSCNT012","lastNamePrinted","0"</v>
       </c>
     </row>
@@ -9088,7 +9440,7 @@
         <v>628</v>
       </c>
       <c r="K181" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51,"R4CNT705","closureLastMonth","20130201"</v>
       </c>
     </row>
@@ -9118,7 +9470,7 @@
         <v>628</v>
       </c>
       <c r="K182" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52,"RSCNT018_01","codCalif1","F0"</v>
       </c>
     </row>
@@ -9148,7 +9500,7 @@
         <v>628</v>
       </c>
       <c r="K183" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>53,"RSCNT019_01","desCalif1","Varios"</v>
       </c>
     </row>
@@ -9178,7 +9530,7 @@
         <v>628</v>
       </c>
       <c r="K184" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54,"RSCNT018_02","codCalif2","F1"</v>
       </c>
     </row>
@@ -9208,7 +9560,7 @@
         <v>628</v>
       </c>
       <c r="K185" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55,"RSCNT019_02","desCalif2","De Primero"</v>
       </c>
     </row>
@@ -9238,7 +9590,7 @@
         <v>628</v>
       </c>
       <c r="K186" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56,"RSCNT018_03","codCalif3","F2"</v>
       </c>
     </row>
@@ -9268,7 +9620,7 @@
         <v>628</v>
       </c>
       <c r="K187" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57,"RSCNT019_03","desCalif3","De Segundo"</v>
       </c>
     </row>
@@ -9298,7 +9650,7 @@
         <v>628</v>
       </c>
       <c r="K188" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58,"RSCNT018_04","codCalif4","F3"</v>
       </c>
     </row>
@@ -9328,7 +9680,7 @@
         <v>628</v>
       </c>
       <c r="K189" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59,"RSCNT019_04","desCalif4","De Tercero"</v>
       </c>
     </row>
@@ -9358,7 +9710,7 @@
         <v>628</v>
       </c>
       <c r="K190" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60,"RSCNT020","channel segment","WEB"</v>
       </c>
     </row>
@@ -9388,7 +9740,7 @@
         <v>628</v>
       </c>
       <c r="K191" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61,"R4CNT003","contCode","R14"</v>
       </c>
     </row>
@@ -9418,7 +9770,7 @@
         <v>628</v>
       </c>
       <c r="K192" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62,"R4CNT004","contSerie","R"</v>
       </c>
     </row>
@@ -9448,7 +9800,7 @@
         <v>628</v>
       </c>
       <c r="K193" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63,"R4CNT023_01","ledgerAccCaja","57000000"</v>
       </c>
     </row>
@@ -9478,7 +9830,7 @@
         <v>628</v>
       </c>
       <c r="K194" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64,"R4CNT023_02","ledgerAccInvi","62700000"</v>
       </c>
     </row>
@@ -9508,7 +9860,7 @@
         <v>628</v>
       </c>
       <c r="K195" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65,"R4CNT023_11","ledgerAccGerVtas","70000000"</v>
       </c>
     </row>
@@ -9538,7 +9890,7 @@
         <v>628</v>
       </c>
       <c r="K196" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66,"R4CNT023_12","ledgerAccServCbtos","70000000"</v>
       </c>
     </row>
@@ -9568,7 +9920,7 @@
         <v>628</v>
       </c>
       <c r="K197" t="str">
-        <f t="shared" ref="K197:K224" si="2">CONCATENATE(B197,C197,D197,E197,F197,G197,H197,I197)</f>
+        <f t="shared" ref="K197:K224" si="3">CONCATENATE(B197,C197,D197,E197,F197,G197,H197,I197)</f>
         <v>67,"R4CNT023_13","ledgerAccPropCam","70000000"</v>
       </c>
     </row>
@@ -9598,7 +9950,7 @@
         <v>628</v>
       </c>
       <c r="K198" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>68,"R4CNT023_14","ledgerAccDescVtas","55599999"</v>
       </c>
     </row>
@@ -9628,7 +9980,7 @@
         <v>628</v>
       </c>
       <c r="K199" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>69,"R4CNT021_01","ivaType1","10.00"</v>
       </c>
     </row>
@@ -9658,7 +10010,7 @@
         <v>628</v>
       </c>
       <c r="K200" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70,"R4CNT022_01","ledgerAccIVA1","47700000"</v>
       </c>
     </row>
@@ -9688,7 +10040,7 @@
         <v>628</v>
       </c>
       <c r="K201" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>71,"R4CNT021_02","ivaType2","10.00"</v>
       </c>
     </row>
@@ -9718,7 +10070,7 @@
         <v>628</v>
       </c>
       <c r="K202" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72,"R4CNT022_02","ledgerAccIVA2","47700000"</v>
       </c>
     </row>
@@ -9748,7 +10100,7 @@
         <v>628</v>
       </c>
       <c r="K203" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>73,"R4CNT021_03","ivaType3","10.00"</v>
       </c>
     </row>
@@ -9778,7 +10130,7 @@
         <v>628</v>
       </c>
       <c r="K204" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74,"R4CNT022_03","ledgerAccIVA3","47700000"</v>
       </c>
     </row>
@@ -9808,7 +10160,7 @@
         <v>628</v>
       </c>
       <c r="K205" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75,"R4CNT201","literalIVA","I.V.A."</v>
       </c>
     </row>
@@ -9838,7 +10190,7 @@
         <v>628</v>
       </c>
       <c r="K206" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>76,"R4CNT018","cadExplot","100"</v>
       </c>
     </row>
@@ -9868,7 +10220,7 @@
         <v>628</v>
       </c>
       <c r="K207" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77,"R4CNT032","cadDept","100"</v>
       </c>
     </row>
@@ -9898,7 +10250,7 @@
         <v>628</v>
       </c>
       <c r="K208" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78,"R4CNT030","covIncomeType","0"</v>
       </c>
     </row>
@@ -9928,7 +10280,7 @@
         <v>628</v>
       </c>
       <c r="K209" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79,"R4CNT031","tipsIncomeType","0"</v>
       </c>
     </row>
@@ -9958,7 +10310,7 @@
         <v>628</v>
       </c>
       <c r="K210" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>80,"R4CNT704","bmpSize","0"</v>
       </c>
     </row>
@@ -9988,7 +10340,7 @@
         <v>628</v>
       </c>
       <c r="K211" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81,"RSCNT017","secuence","1C 28 45 06 00 3E 02 20 20 31 05"</v>
       </c>
     </row>
@@ -10018,7 +10370,7 @@
         <v>628</v>
       </c>
       <c r="K212" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82,"RSCNT012","pageLength","0"</v>
       </c>
     </row>
@@ -10048,7 +10400,7 @@
         <v>628</v>
       </c>
       <c r="K213" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>83,"RSCNT013","skipHeaderLines","0"</v>
       </c>
     </row>
@@ -10078,7 +10430,7 @@
         <v>628</v>
       </c>
       <c r="K214" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84,"RSCNT014","leftTab","0"</v>
       </c>
     </row>
@@ -10108,7 +10460,7 @@
         <v>628</v>
       </c>
       <c r="K215" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85,"RSCNT015","commandPortPrt1","1111"</v>
       </c>
     </row>
@@ -10138,7 +10490,7 @@
         <v>628</v>
       </c>
       <c r="K216" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86,"RSCNT016","commandPortPrt2","1111"</v>
       </c>
     </row>
@@ -10166,7 +10518,7 @@
         <v>628</v>
       </c>
       <c r="K217" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87,"RXCNT002","ipLVDE",""</v>
       </c>
     </row>
@@ -10194,7 +10546,7 @@
         <v>628</v>
       </c>
       <c r="K218" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88,"RXCNT003","ipHelp",""</v>
       </c>
     </row>
@@ -10222,7 +10574,7 @@
         <v>628</v>
       </c>
       <c r="K219" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89,"RXCNT004","ipCCC",""</v>
       </c>
     </row>
@@ -10250,7 +10602,7 @@
         <v>628</v>
       </c>
       <c r="K220" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90,"RXCNT005","ipAlternative",""</v>
       </c>
     </row>
@@ -10278,7 +10630,7 @@
         <v>628</v>
       </c>
       <c r="K221" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91,"R4CNT025","sendEmail",""</v>
       </c>
     </row>
@@ -10306,7 +10658,7 @@
         <v>628</v>
       </c>
       <c r="K222" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>92,"R4CNT026","sendService",""</v>
       </c>
     </row>
@@ -10334,7 +10686,7 @@
         <v>628</v>
       </c>
       <c r="K223" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>93,"R4CNT027","sendLogin",""</v>
       </c>
     </row>
@@ -10362,7 +10714,7 @@
         <v>628</v>
       </c>
       <c r="K224" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>94,"R4CNT028","sendPsw",""</v>
       </c>
     </row>

</xml_diff>

<commit_message>
acabado el diseño de las pestañas de configuración
</commit_message>
<xml_diff>
--- a/doc/ParametrosConfig.xlsx
+++ b/doc/ParametrosConfig.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="652">
   <si>
     <t>RES14CNT_GN</t>
   </si>
@@ -2004,6 +2004,12 @@
   </si>
   <si>
     <t>R4CNT141</t>
+  </si>
+  <si>
+    <t>precioxPax</t>
+  </si>
+  <si>
+    <t>Línea precion por Pax</t>
   </si>
 </sst>
 </file>
@@ -2480,8 +2486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F134" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H141" sqref="H141"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4410,6 +4416,24 @@
         <v>229</v>
       </c>
       <c r="I31" s="3"/>
+      <c r="J31" s="20">
+        <v>29</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N31" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>651</v>
+      </c>
       <c r="R31" s="2" t="s">
         <v>249</v>
       </c>

</xml_diff>

<commit_message>
añadido comportamiento para página de configuración.
</commit_message>
<xml_diff>
--- a/doc/ParametrosConfig.xlsx
+++ b/doc/ParametrosConfig.xlsx
@@ -10,6 +10,7 @@
     <sheet name="ParamConfig" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -2486,8 +2487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2649,7 +2650,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>123456</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>26</v>
@@ -2727,7 +2728,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>234567</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>38</v>
@@ -2802,7 +2803,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>345678</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>48</v>
@@ -2877,7 +2878,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>456789</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>58</v>
@@ -2951,7 +2952,9 @@
       <c r="F7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="18">
+        <v>56789</v>
+      </c>
       <c r="H7" s="17" t="s">
         <v>66</v>
       </c>

</xml_diff>